<commit_message>
doi server 4.90 = > 4.143, them IP Wan
</commit_message>
<xml_diff>
--- a/Tong hop svr  30-10-2013.xlsx
+++ b/Tong hop svr  30-10-2013.xlsx
@@ -13,7 +13,8 @@
     <sheet name="SMS-Voice" sheetId="6" r:id="rId4"/>
     <sheet name="Liên hệ" sheetId="12" r:id="rId5"/>
     <sheet name="Thay đổi SVR" sheetId="13" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId7"/>
+    <sheet name="Sheet" sheetId="15" r:id="rId7"/>
+    <sheet name="Cloud" sheetId="16" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VDC-TL'!$L$1:$L$1262</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10991" uniqueCount="4378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11007" uniqueCount="4378">
   <si>
     <t>222.255.27.129</t>
   </si>
@@ -17066,6 +17067,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="23" borderId="7" xfId="38" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -17129,25 +17131,24 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="22" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -17674,8 +17675,8 @@
   <dimension ref="A1:IP1262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A904" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H913" sqref="H913"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17699,23 +17700,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:250" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="689" t="s">
+      <c r="A1" s="690" t="s">
         <v>2475</v>
       </c>
-      <c r="B1" s="690"/>
-      <c r="C1" s="690"/>
-      <c r="D1" s="690"/>
-      <c r="E1" s="690"/>
-      <c r="F1" s="690"/>
-      <c r="G1" s="690"/>
-      <c r="H1" s="690"/>
-      <c r="I1" s="690"/>
-      <c r="J1" s="690"/>
-      <c r="K1" s="690"/>
-      <c r="L1" s="690"/>
-      <c r="M1" s="690"/>
-      <c r="N1" s="690"/>
-      <c r="O1" s="690"/>
+      <c r="B1" s="691"/>
+      <c r="C1" s="691"/>
+      <c r="D1" s="691"/>
+      <c r="E1" s="691"/>
+      <c r="F1" s="691"/>
+      <c r="G1" s="691"/>
+      <c r="H1" s="691"/>
+      <c r="I1" s="691"/>
+      <c r="J1" s="691"/>
+      <c r="K1" s="691"/>
+      <c r="L1" s="691"/>
+      <c r="M1" s="691"/>
+      <c r="N1" s="691"/>
+      <c r="O1" s="691"/>
     </row>
     <row r="2" spans="1:250" s="301" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="537" t="s">
@@ -62168,27 +62169,27 @@
     </row>
     <row r="1251" spans="1:24" s="12" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1251" s="26"/>
-      <c r="B1251" s="718" t="s">
+      <c r="B1251" s="689" t="s">
         <v>4370</v>
       </c>
       <c r="C1251" s="92"/>
-      <c r="D1251" s="718" t="s">
+      <c r="D1251" s="689" t="s">
         <v>4374</v>
       </c>
-      <c r="E1251" s="718" t="s">
+      <c r="E1251" s="689" t="s">
         <v>4373</v>
       </c>
-      <c r="F1251" s="718" t="s">
+      <c r="F1251" s="689" t="s">
         <v>4375</v>
       </c>
-      <c r="G1251" s="718" t="s">
+      <c r="G1251" s="689" t="s">
         <v>4372</v>
       </c>
       <c r="H1251" s="101"/>
       <c r="I1251" s="101"/>
       <c r="J1251" s="101"/>
       <c r="K1251" s="92"/>
-      <c r="L1251" s="718" t="s">
+      <c r="L1251" s="689" t="s">
         <v>4371</v>
       </c>
       <c r="M1251" s="26" t="s">
@@ -62480,22 +62481,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:249" s="3" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="689" t="s">
+      <c r="A1" s="690" t="s">
         <v>2475</v>
       </c>
-      <c r="B1" s="690"/>
-      <c r="C1" s="690"/>
-      <c r="D1" s="690"/>
-      <c r="E1" s="690"/>
-      <c r="F1" s="690"/>
-      <c r="G1" s="690"/>
-      <c r="H1" s="690"/>
-      <c r="I1" s="690"/>
-      <c r="J1" s="690"/>
-      <c r="K1" s="690"/>
-      <c r="L1" s="690"/>
-      <c r="M1" s="690"/>
-      <c r="N1" s="690"/>
+      <c r="B1" s="691"/>
+      <c r="C1" s="691"/>
+      <c r="D1" s="691"/>
+      <c r="E1" s="691"/>
+      <c r="F1" s="691"/>
+      <c r="G1" s="691"/>
+      <c r="H1" s="691"/>
+      <c r="I1" s="691"/>
+      <c r="J1" s="691"/>
+      <c r="K1" s="691"/>
+      <c r="L1" s="691"/>
+      <c r="M1" s="691"/>
+      <c r="N1" s="691"/>
     </row>
     <row r="2" spans="1:249" s="301" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="537" t="s">
@@ -63056,67 +63057,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="706" t="s">
+      <c r="A1" s="707" t="s">
         <v>719</v>
       </c>
-      <c r="B1" s="708" t="s">
+      <c r="B1" s="709" t="s">
         <v>720</v>
       </c>
-      <c r="C1" s="710" t="s">
+      <c r="C1" s="711" t="s">
         <v>746</v>
       </c>
-      <c r="D1" s="710" t="s">
+      <c r="D1" s="711" t="s">
         <v>722</v>
       </c>
-      <c r="E1" s="710" t="s">
+      <c r="E1" s="711" t="s">
         <v>723</v>
       </c>
-      <c r="F1" s="704" t="s">
+      <c r="F1" s="705" t="s">
         <v>724</v>
       </c>
-      <c r="G1" s="702" t="s">
+      <c r="G1" s="703" t="s">
         <v>725</v>
       </c>
-      <c r="H1" s="702" t="s">
+      <c r="H1" s="703" t="s">
         <v>726</v>
       </c>
-      <c r="I1" s="702" t="s">
+      <c r="I1" s="703" t="s">
         <v>727</v>
       </c>
-      <c r="J1" s="702" t="s">
+      <c r="J1" s="703" t="s">
         <v>728</v>
       </c>
-      <c r="K1" s="700" t="s">
+      <c r="K1" s="701" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="707"/>
-      <c r="B2" s="709"/>
-      <c r="C2" s="711"/>
-      <c r="D2" s="711"/>
-      <c r="E2" s="711"/>
-      <c r="F2" s="705"/>
-      <c r="G2" s="703"/>
-      <c r="H2" s="703"/>
-      <c r="I2" s="703"/>
-      <c r="J2" s="703"/>
-      <c r="K2" s="701"/>
+      <c r="A2" s="708"/>
+      <c r="B2" s="710"/>
+      <c r="C2" s="712"/>
+      <c r="D2" s="712"/>
+      <c r="E2" s="712"/>
+      <c r="F2" s="706"/>
+      <c r="G2" s="704"/>
+      <c r="H2" s="704"/>
+      <c r="I2" s="704"/>
+      <c r="J2" s="704"/>
+      <c r="K2" s="702"/>
     </row>
     <row r="3" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="694" t="s">
+      <c r="A3" s="695" t="s">
         <v>1884</v>
       </c>
-      <c r="B3" s="695"/>
-      <c r="C3" s="695"/>
-      <c r="D3" s="695"/>
-      <c r="E3" s="695"/>
-      <c r="F3" s="695"/>
-      <c r="G3" s="695"/>
-      <c r="H3" s="695"/>
-      <c r="I3" s="695"/>
-      <c r="J3" s="695"/>
-      <c r="K3" s="696"/>
+      <c r="B3" s="696"/>
+      <c r="C3" s="696"/>
+      <c r="D3" s="696"/>
+      <c r="E3" s="696"/>
+      <c r="F3" s="696"/>
+      <c r="G3" s="696"/>
+      <c r="H3" s="696"/>
+      <c r="I3" s="696"/>
+      <c r="J3" s="696"/>
+      <c r="K3" s="697"/>
     </row>
     <row r="4" spans="1:11" s="12" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="350">
@@ -63174,19 +63175,19 @@
       <c r="K6" s="61"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="697" t="s">
+      <c r="A7" s="698" t="s">
         <v>1801</v>
       </c>
-      <c r="B7" s="698"/>
-      <c r="C7" s="698"/>
-      <c r="D7" s="698"/>
-      <c r="E7" s="698"/>
-      <c r="F7" s="698"/>
-      <c r="G7" s="698"/>
-      <c r="H7" s="698"/>
-      <c r="I7" s="698"/>
-      <c r="J7" s="698"/>
-      <c r="K7" s="699"/>
+      <c r="B7" s="699"/>
+      <c r="C7" s="699"/>
+      <c r="D7" s="699"/>
+      <c r="E7" s="699"/>
+      <c r="F7" s="699"/>
+      <c r="G7" s="699"/>
+      <c r="H7" s="699"/>
+      <c r="I7" s="699"/>
+      <c r="J7" s="699"/>
+      <c r="K7" s="700"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="61"/>
@@ -63225,19 +63226,19 @@
       <c r="K9" s="61"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="697" t="s">
+      <c r="A10" s="698" t="s">
         <v>1806</v>
       </c>
-      <c r="B10" s="698"/>
-      <c r="C10" s="698"/>
-      <c r="D10" s="698"/>
-      <c r="E10" s="698"/>
-      <c r="F10" s="698"/>
-      <c r="G10" s="698"/>
-      <c r="H10" s="698"/>
-      <c r="I10" s="698"/>
-      <c r="J10" s="698"/>
-      <c r="K10" s="699"/>
+      <c r="B10" s="699"/>
+      <c r="C10" s="699"/>
+      <c r="D10" s="699"/>
+      <c r="E10" s="699"/>
+      <c r="F10" s="699"/>
+      <c r="G10" s="699"/>
+      <c r="H10" s="699"/>
+      <c r="I10" s="699"/>
+      <c r="J10" s="699"/>
+      <c r="K10" s="700"/>
     </row>
     <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="61"/>
@@ -63317,19 +63318,19 @@
       <c r="K15" s="61"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="697" t="s">
+      <c r="A16" s="698" t="s">
         <v>1880</v>
       </c>
-      <c r="B16" s="698"/>
-      <c r="C16" s="698"/>
-      <c r="D16" s="698"/>
-      <c r="E16" s="698"/>
-      <c r="F16" s="698"/>
-      <c r="G16" s="698"/>
-      <c r="H16" s="698"/>
-      <c r="I16" s="698"/>
-      <c r="J16" s="698"/>
-      <c r="K16" s="699"/>
+      <c r="B16" s="699"/>
+      <c r="C16" s="699"/>
+      <c r="D16" s="699"/>
+      <c r="E16" s="699"/>
+      <c r="F16" s="699"/>
+      <c r="G16" s="699"/>
+      <c r="H16" s="699"/>
+      <c r="I16" s="699"/>
+      <c r="J16" s="699"/>
+      <c r="K16" s="700"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="61"/>
@@ -63372,19 +63373,19 @@
       <c r="K18" s="61"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="691" t="s">
+      <c r="A20" s="692" t="s">
         <v>1938</v>
       </c>
-      <c r="B20" s="692"/>
-      <c r="C20" s="692"/>
-      <c r="D20" s="692"/>
-      <c r="E20" s="692"/>
-      <c r="F20" s="692"/>
-      <c r="G20" s="692"/>
-      <c r="H20" s="692"/>
-      <c r="I20" s="692"/>
-      <c r="J20" s="692"/>
-      <c r="K20" s="693"/>
+      <c r="B20" s="693"/>
+      <c r="C20" s="693"/>
+      <c r="D20" s="693"/>
+      <c r="E20" s="693"/>
+      <c r="F20" s="693"/>
+      <c r="G20" s="693"/>
+      <c r="H20" s="693"/>
+      <c r="I20" s="693"/>
+      <c r="J20" s="693"/>
+      <c r="K20" s="694"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="61"/>
@@ -63480,10 +63481,10 @@
       <c r="F3"/>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="712" t="s">
+      <c r="A4" s="717" t="s">
         <v>719</v>
       </c>
-      <c r="B4" s="713" t="s">
+      <c r="B4" s="718" t="s">
         <v>720</v>
       </c>
       <c r="C4" s="714" t="s">
@@ -63495,37 +63496,37 @@
       <c r="E4" s="714" t="s">
         <v>508</v>
       </c>
-      <c r="F4" s="717" t="s">
+      <c r="F4" s="715" t="s">
         <v>724</v>
       </c>
-      <c r="G4" s="715" t="s">
+      <c r="G4" s="716" t="s">
         <v>725</v>
       </c>
-      <c r="H4" s="715" t="s">
+      <c r="H4" s="716" t="s">
         <v>726</v>
       </c>
-      <c r="I4" s="715" t="s">
+      <c r="I4" s="716" t="s">
         <v>727</v>
       </c>
       <c r="J4" s="714" t="s">
         <v>509</v>
       </c>
-      <c r="K4" s="716" t="s">
+      <c r="K4" s="713" t="s">
         <v>729</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="712"/>
-      <c r="B5" s="713"/>
+      <c r="A5" s="717"/>
+      <c r="B5" s="718"/>
       <c r="C5" s="714"/>
       <c r="D5" s="714"/>
       <c r="E5" s="714"/>
-      <c r="F5" s="717"/>
-      <c r="G5" s="715"/>
-      <c r="H5" s="715"/>
-      <c r="I5" s="715"/>
+      <c r="F5" s="715"/>
+      <c r="G5" s="716"/>
+      <c r="H5" s="716"/>
+      <c r="I5" s="716"/>
       <c r="J5" s="714"/>
-      <c r="K5" s="716"/>
+      <c r="K5" s="713"/>
     </row>
     <row r="6" spans="1:13" s="8" customFormat="1" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
@@ -63780,17 +63781,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="I4:I5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="J4:J5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I4:I5"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
@@ -66869,4 +66870,88 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="690" t="s">
+        <v>2475</v>
+      </c>
+      <c r="B1" s="691"/>
+      <c r="C1" s="691"/>
+      <c r="D1" s="691"/>
+      <c r="E1" s="691"/>
+      <c r="F1" s="691"/>
+      <c r="G1" s="691"/>
+      <c r="H1" s="691"/>
+      <c r="I1" s="691"/>
+      <c r="J1" s="691"/>
+      <c r="K1" s="691"/>
+      <c r="L1" s="691"/>
+      <c r="M1" s="691"/>
+      <c r="N1" s="691"/>
+      <c r="O1" s="691"/>
+    </row>
+    <row r="2" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="537" t="s">
+        <v>719</v>
+      </c>
+      <c r="B2" s="538" t="s">
+        <v>720</v>
+      </c>
+      <c r="C2" s="537" t="s">
+        <v>746</v>
+      </c>
+      <c r="D2" s="537" t="s">
+        <v>722</v>
+      </c>
+      <c r="E2" s="537" t="s">
+        <v>747</v>
+      </c>
+      <c r="F2" s="536" t="s">
+        <v>724</v>
+      </c>
+      <c r="G2" s="537" t="s">
+        <v>725</v>
+      </c>
+      <c r="H2" s="537" t="s">
+        <v>726</v>
+      </c>
+      <c r="I2" s="537" t="s">
+        <v>2500</v>
+      </c>
+      <c r="J2" s="537" t="s">
+        <v>727</v>
+      </c>
+      <c r="K2" s="537" t="s">
+        <v>728</v>
+      </c>
+      <c r="L2" s="535" t="s">
+        <v>748</v>
+      </c>
+      <c r="M2" s="537" t="s">
+        <v>729</v>
+      </c>
+      <c r="N2" s="537" t="s">
+        <v>3187</v>
+      </c>
+      <c r="O2" s="534" t="s">
+        <v>2484</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>